<commit_message>
Fixed 2023 champions name
</commit_message>
<xml_diff>
--- a/resources/nba-awards.xlsx
+++ b/resources/nba-awards.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan_\OneDrive\Área de Trabalho\Data Engineering\NBA Recap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luan_\OneDrive\Área de Trabalho\Data Engineering\NBA Recap\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28786304-4D78-4FA0-A8BD-24A608B5AA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62D8FD7-5E55-48C6-AC17-42C96057968A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1060,7 +1060,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1213,6 +1213,14 @@
     <font>
       <u/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1581,9 +1589,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1943,7 +1953,7 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,7 +2003,7 @@
         <v>2023</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="D2" t="str">
         <f>VLOOKUP(A2,'Final MVP'!A:B,2,0)</f>
@@ -2027,7 +2037,7 @@
       <c r="B3" s="1">
         <v>2022</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>314</v>
       </c>
       <c r="D3" t="str">
@@ -2794,7 +2804,7 @@
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="8">
         <v>2000</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -3724,7 +3734,7 @@
   <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5513,7 +5523,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
@@ -5653,7 +5663,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -5661,7 +5671,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -5669,7 +5679,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -5677,7 +5687,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -5685,7 +5695,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -5693,7 +5703,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -5701,7 +5711,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -5709,7 +5719,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -5717,16 +5727,15 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -5734,7 +5743,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -5742,7 +5751,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -5750,7 +5759,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>45</v>
       </c>
@@ -5758,7 +5767,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
@@ -5766,7 +5775,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>48</v>
       </c>
@@ -5774,7 +5783,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>